<commit_message>
Correção nas chaves estrangeiras do movimento dos paciente
</commit_message>
<xml_diff>
--- a/bd/banco dados medibase.xlsx
+++ b/bd/banco dados medibase.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Notebook\Documents\Aulas\Proz Tech\projeto_proz_turma14\bd\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEF63609-4C04-4054-B5E1-76EAC30287E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38A52EA9-3D59-4B6E-8DD5-E411B91D7547}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{5F268087-FE2C-43B7-BC5D-30D8953797CB}"/>
   </bookViews>
@@ -304,199 +304,199 @@
     <t xml:space="preserve">    (19, 22, 12, 9, '2023-11-09', '14:30:00', 'A', 'Dermatology consultation. Prescription provided.');</t>
   </si>
   <si>
+    <t>CREATE TABLE "medico" (</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "med_id" SERIAL PRIMARY KEY,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "med_nome" VARCHAR(100) NOT NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "med_datanasc" DATE NOT NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "med_endereco" VARCHAR(100),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "med_cidade" VARCHAR(50),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "med_bairro" VARCHAR(50),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "med_crm" INT UNIQUE NOT NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "med_uf_crm" VARCHAR(2) NOT NULL,</t>
+  </si>
+  <si>
+    <t>CREATE TABLE "especialidade" (</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "esp_id" SERIAL PRIMARY KEY,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "esp_nome_especialidade" VARCHAR(100) NOT NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "esp_codigo_especialidade" SMALLINT UNIQUE NOT NULL,</t>
+  </si>
+  <si>
+    <t>CREATE TABLE "medico_especialidade" (</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "med_esp_id" SERIAL PRIMARY KEY,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "fk_med_id" INT NOT NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "fk_esp_id" INT NOT NULL,</t>
+  </si>
+  <si>
+    <t>CREATE TABLE "convenio" (</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "con_id" SERIAL PRIMARY KEY,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "con_nome_convenio" VARCHAR(50) NOT NULL,</t>
+  </si>
+  <si>
+    <t>CREATE TABLE "paciente" (</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "pac_prontuario" SERIAL PRIMARY KEY,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "pac_nome" VARCHAR(100) NOT NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "pac_datanasc" DATE NOT NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "pac_endereco" VARCHAR(100),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "pac_cidade" VARCHAR(50),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "pac_bairro" VARCHAR(50),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "pac_nome_mae" VARCHAR(100),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "pac_nome_pai" VARCHAR(100),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "pac_responsavel" VARCHAR(100) NOT NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "fk_con_id" INT NOT NULL,</t>
+  </si>
+  <si>
+    <t>CREATE TABLE "mov_consulta_paciente" (</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "mov_id" SERIAL PRIMARY KEY,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "fk_pac_prontuario" INT NOT NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "mov_data_atende" DATE NOT NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "mov_hora_atende" TIME NOT NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "med_cpf" CHAR(14) UNIQUE NOT NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "med_rg" CHAR(12),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "med_apelido" CHAR(20),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "med_cep" CHAR(10),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "med_uf_medico" CHAR(2),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "med_fone" CHAR(20) NOT NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "med_ativo" CHAR(1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "esp_ativo" CHAR(1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "med_esp_ativo" CHAR(1) NOT NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  CONSTRAINT "fk_medico_especialidade_medico" FOREIGN KEY ("fk_med_id") REFERENCES "medico" ("med_id"),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  CONSTRAINT "fk_medico_especialidade_especialidade" FOREIGN KEY ("fk_esp_id") REFERENCES "especialidade" ("esp_id")</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "con_tipo_plano" CHAR(3) NOT NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "con_fone" CHAR(20) NOT NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "con_ativo" CHAR(1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "pac_cpf" CHAR(14) UNIQUE NOT NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "pac_rg" CHAR(12),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "pac_sexo" CHAR(1) NOT NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "pac_estado_civil" CHAR(15),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "pac_cep" CHAR(10),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "pac_fone" CHAR(20) NOT NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "pac_ativo" CHAR(1),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  CONSTRAINT "fk_paciente_convenio" FOREIGN KEY ("fk_con_id") REFERENCES "convenio" ("con_id")</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "mov_ativo" CHAR(1),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "mov_evolucao_medica" TEXT,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  CONSTRAINT "fk_mov_consulta_paciente_paciente" FOREIGN KEY ("fk_pac_prontuario") REFERENCES "paciente" ("pac_prontuario"),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  CONSTRAINT "fk_mov_consulta_paciente_medico" FOREIGN KEY ("fk_med_id") REFERENCES "medico" ("med_id"),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  CONSTRAINT "fk_mov_consulta_paciente_especialidade" FOREIGN KEY ("fk_esp_id") REFERENCES "especialidade" ("esp_id"),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  CONSTRAINT "fk_mov_consulta_paciente_convenio" FOREIGN KEY ("fk_con_id") REFERENCES "convenio" ("con_id")</t>
+  </si>
+  <si>
     <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>CREATE TABLE "medico" (</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "med_id" SERIAL PRIMARY KEY,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "med_nome" VARCHAR(100) NOT NULL,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "med_datanasc" DATE NOT NULL,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "med_cpf" "CHAR (14)" UNIQUE NOT NULL,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "med_rg" "CHAR (12)",</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "med_apelido" "CHAR (20)",</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "med_cep" "CHAR (10)",</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "med_endereco" VARCHAR(100),</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "med_cidade" VARCHAR(50),</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "med_uf_medico" "CHAR (2)",</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "med_bairro" VARCHAR(50),</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "med_fone" "CHAR (20)" NOT NULL,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "med_crm" INT UNIQUE NOT NULL,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "med_uf_crm" VARCHAR(2) NOT NULL,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "med_ativo" "char (1)"</t>
-  </si>
-  <si>
-    <t>CREATE TABLE "especialidade" (</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "esp_id" SERIAL PRIMARY KEY,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "esp_nome_especialidade" VARCHAR(100) NOT NULL,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "esp_codigo_especialidade" SMALLINT UNIQUE NOT NULL,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "esp_ativo" "char (1)"</t>
-  </si>
-  <si>
-    <t>CREATE TABLE "medico_especialidade" (</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "med_esp_id" SERIAL PRIMARY KEY,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "fk_med_id" INT NOT NULL,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "fk_esp_id" INT NOT NULL,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "med_esp_ativo" "char (1)" NOT NULL</t>
-  </si>
-  <si>
-    <t>CREATE TABLE "convenio" (</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "con_id" SERIAL PRIMARY KEY,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "con_nome_convenio" VARCHAR(50) NOT NULL,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "con_tipo_plano" "CHAR (3)" NOT NULL,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "con_fone" "CHAR (20)" NOT NULL,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "con_ativo" "char (1)"</t>
-  </si>
-  <si>
-    <t>CREATE TABLE "paciente" (</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "pac_prontuario" SERIAL PRIMARY KEY,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "pac_nome" VARCHAR(100) NOT NULL,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "pac_datanasc" DATE NOT NULL,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "pac_cpf" "CHAR (14)" UNIQUE NOT NULL,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "pac_rg" "CHAR (12)",</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "pac_sexo" "CHAR (1)" NOT NULL,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "pac_estado_civil" "CHAR (15)",</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "pac_endereco" VARCHAR(100),</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "pac_cidade" VARCHAR(50),</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "pac_bairro" VARCHAR(50),</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "pac_cep" "CHAR (10)",</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "pac_fone" "CHAR (20)" NOT NULL,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "pac_nome_mae" VARCHAR(100),</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "pac_nome_pai" VARCHAR(100),</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "pac_responsavel" VARCHAR(100) NOT NULL,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "fk_con_id" INT NOT NULL,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "pac_ativo" "char (1)"</t>
-  </si>
-  <si>
-    <t>CREATE TABLE "mov_consulta_paciente" (</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "mov_id" SERIAL PRIMARY KEY,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "fk_pac_prontuario" INT NOT NULL,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "mov_data_atende" DATE NOT NULL,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "mov_hora_atende" TIME NOT NULL,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "mov_ativo" "char (1)",</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "mov_evolucao_medica" TEXT</t>
-  </si>
-  <si>
-    <t>ALTER TABLE "medico_especialidade" ADD CONSTRAINT "fk_med_id" FOREIGN KEY ("fk_med_id") REFERENCES "medico" ("med_id");</t>
-  </si>
-  <si>
-    <t>ALTER TABLE "medico_especialidade" ADD CONSTRAINT "fk_esp_id" FOREIGN KEY ("fk_esp_id") REFERENCES "especialidade" ("esp_id");</t>
-  </si>
-  <si>
-    <t>ALTER TABLE "paciente" ADD CONSTRAINT "fk_con_id" FOREIGN KEY ("fk_con_id") REFERENCES "convenio" ("con_id");</t>
-  </si>
-  <si>
-    <t>ALTER TABLE "mov_consulta_paciente" ADD FOREIGN KEY ("fk_pac_prontuario") REFERENCES "paciente" ("pac_prontuario");</t>
-  </si>
-  <si>
-    <t>ALTER TABLE "mov_consulta_paciente" ADD FOREIGN KEY ("fk_med_id") REFERENCES "medico" ("med_id");</t>
-  </si>
-  <si>
-    <t>ALTER TABLE "mov_consulta_paciente" ADD FOREIGN KEY ("fk_esp_id") REFERENCES "especialidade" ("esp_id");</t>
-  </si>
-  <si>
-    <t>ALTER TABLE "mov_consulta_paciente" ADD FOREIGN KEY ("fk_con_id") REFERENCES "convenio" ("con_id");</t>
   </si>
 </sst>
 </file>
@@ -882,7 +882,7 @@
   <dimension ref="A1:D87"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -901,87 +901,87 @@
     </row>
     <row r="2" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>88</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>93</v>
+        <v>124</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>94</v>
+        <v>125</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>95</v>
+        <v>126</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>96</v>
+        <v>127</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>99</v>
+        <v>128</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>101</v>
+        <v>129</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>104</v>
+        <v>130</v>
       </c>
     </row>
     <row r="19" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
@@ -994,27 +994,27 @@
     </row>
     <row r="21" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
     </row>
     <row r="22" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
     </row>
     <row r="23" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
     </row>
     <row r="24" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
     </row>
     <row r="25" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>109</v>
+        <v>131</v>
       </c>
     </row>
     <row r="26" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
@@ -1027,280 +1027,284 @@
     </row>
     <row r="28" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
     </row>
     <row r="29" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
     </row>
     <row r="30" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
     </row>
     <row r="31" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
     </row>
     <row r="32" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>114</v>
+        <v>132</v>
       </c>
     </row>
     <row r="33" spans="1:2" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.25"/>
+        <v>133</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>134</v>
+      </c>
+    </row>
     <row r="35" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
-        <v>115</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A36" s="2" t="s">
-        <v>116</v>
-      </c>
+      <c r="A36" s="2"/>
     </row>
     <row r="37" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>120</v>
+        <v>135</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>1</v>
+        <v>136</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A42" s="3"/>
+      <c r="A42" s="3" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="43" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>121</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A44" s="3" t="s">
-        <v>122</v>
-      </c>
+      <c r="A44" s="3"/>
     </row>
     <row r="45" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>123</v>
+        <v>108</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="B47" s="1"/>
     </row>
     <row r="48" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>126</v>
+        <v>111</v>
       </c>
     </row>
     <row r="49" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>127</v>
+        <v>138</v>
       </c>
     </row>
     <row r="50" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>128</v>
+        <v>139</v>
       </c>
     </row>
     <row r="51" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>129</v>
+        <v>140</v>
       </c>
     </row>
     <row r="52" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>130</v>
+        <v>141</v>
       </c>
     </row>
     <row r="53" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>131</v>
+        <v>112</v>
       </c>
     </row>
     <row r="54" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>132</v>
+        <v>113</v>
       </c>
     </row>
     <row r="55" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>133</v>
+        <v>114</v>
       </c>
     </row>
     <row r="56" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
     </row>
     <row r="57" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
     </row>
     <row r="58" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>136</v>
+        <v>115</v>
       </c>
     </row>
     <row r="59" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>137</v>
+        <v>116</v>
       </c>
     </row>
     <row r="60" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
-        <v>138</v>
+        <v>117</v>
       </c>
     </row>
     <row r="61" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
-        <v>1</v>
+        <v>118</v>
       </c>
     </row>
     <row r="62" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A62" s="3"/>
+      <c r="A62" s="3" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="63" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
     </row>
     <row r="64" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
-        <v>140</v>
+        <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A65" s="3" t="s">
-        <v>141</v>
-      </c>
+      <c r="A65" s="3"/>
     </row>
     <row r="66" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
     </row>
     <row r="67" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
     </row>
     <row r="68" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
-        <v>137</v>
+        <v>121</v>
       </c>
     </row>
     <row r="69" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
-        <v>142</v>
+        <v>103</v>
       </c>
     </row>
     <row r="70" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
-        <v>143</v>
+        <v>104</v>
       </c>
     </row>
     <row r="71" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
-        <v>144</v>
+        <v>118</v>
       </c>
     </row>
     <row r="72" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
-        <v>145</v>
+        <v>122</v>
       </c>
     </row>
     <row r="73" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
-        <v>1</v>
+        <v>123</v>
       </c>
     </row>
     <row r="74" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A74" s="2"/>
+      <c r="A74" s="2" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="75" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="76" spans="1:1" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.25"/>
+        <v>147</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A76" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
     <row r="77" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="78" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A78" s="3"/>
+      <c r="A78" s="3" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="79" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
     </row>
     <row r="80" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A80" s="2"/>
+      <c r="A80" s="2" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="81" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A81" s="2" t="s">
-        <v>149</v>
-      </c>
+      <c r="A81" s="2"/>
     </row>
     <row r="82" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A82" s="2"/>
     </row>
     <row r="83" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A83" s="3" t="s">
-        <v>150</v>
-      </c>
+      <c r="A83" s="3"/>
     </row>
     <row r="84" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A84" s="2"/>
     </row>
     <row r="85" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A85" s="2" t="s">
-        <v>151</v>
-      </c>
+      <c r="A85" s="2"/>
     </row>
     <row r="86" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A86" s="2"/>
     </row>
     <row r="87" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A87" s="2" t="s">
-        <v>152</v>
-      </c>
+      <c r="A87" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Alteração da tabela paciente dividindo em 2 tabelas endereço e telefone
</commit_message>
<xml_diff>
--- a/bd/banco dados medibase.xlsx
+++ b/bd/banco dados medibase.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Notebook\Documents\Aulas\Proz Tech\projeto_proz_turma14\bd\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38A52EA9-3D59-4B6E-8DD5-E411B91D7547}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF262247-1589-40E9-9667-51F63319CBD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{5F268087-FE2C-43B7-BC5D-30D8953797CB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{5F268087-FE2C-43B7-BC5D-30D8953797CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Banco Dados E Tabelas" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="166">
   <si>
     <t>Nome banco de dados: medibase</t>
   </si>
@@ -49,105 +49,9 @@
     <t>-- Inserir 10 registros para a tabela medico</t>
   </si>
   <si>
-    <t>INSERT INTO medico (med_nome, med_datanasc, med_cpf, med_rg, med_apelido, med_cep, med_endereco, med_cidade, med_uf_medico, med_bairro, med_fone, med_crm, med_uf_crm, med_ativo)</t>
-  </si>
-  <si>
     <t>VALUES</t>
   </si>
   <si>
-    <t xml:space="preserve">    ('Dr. João', '1980-01-01', '123.456.789-01', '123456789012', 'Dr. J', '12345-678', 'Rua Principal, 123', 'Cidade A', 'UF', 'Bairro A', '(11) 98765-4321', 12345, 'SP', 'A'),</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    ('Dra. Maria', '1975-05-15', '987.654.321-01', '987654321012', 'Dra. M', '54321-876', 'Avenida Secundária, 456', 'Cidade B', 'UF', 'Bairro B', '(11) 8765-4321', 54321, 'RJ', 'A'),</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    ('Dr. Carlos', '1988-08-08', '111.222.333-44', '111222333444', 'Dr. C', '87654-321', 'Rua X, 789', 'Cidade C', 'UF', 'Bairro C', '(11) 7654-3210', 67890, 'SP', 'A'),</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    ('Dra. Ana', '1990-03-12', '555.666.777-88', '555666777888', 'Dra. A', '56789-012', 'Rua Y, 987', 'Cidade D', 'UF', 'Bairro D', '(22) 5432-1098', 98765, 'RJ', 'A'),</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    ('Dr. Roberto', '1985-11-25', '777.888.999-00', '777888999000', 'Dr. R', '34567-890', 'Rua Z, 543', 'Cidade E', 'UF', 'Bairro E', '(22) 4321-9876', 34567, 'SP', 'A'),</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    ('Dra. Paula', '1972-09-30', '444.555.666-77', '444555666777', 'Dra. P', '23456-789', 'Avenida W, 876', 'Cidade F', 'UF', 'Bairro F', '(11) 8765-4321', 87654, 'RJ', 'A'),</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    ('Dr. Ricardo', '1982-06-18', '666.777.888-99', '666777888999', 'Dr. R', '12345-678', 'Rua K, 123', 'Cidade G', 'UF', 'Bairro G', '(22) 9876-5432', 23456, 'SP', 'A'),</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    ('Dra. Silvia', '1978-04-05', '999.000.111-22', '999000111222', 'Dra. S', '54321-876', 'Avenida L, 987', 'Cidade H', 'UF', 'Bairro H', '(11) 5432-1098', 78901, 'RJ', 'A'),</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    ('Dr. Marcos', '1987-02-14', '333.444.555-66', '333444555666', 'Dr. M', '87654-321', 'Rua M, 543', 'Cidade I', 'UF', 'Bairro I', '(22) 8765-4321', 12349, 'SP', 'A'),</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    ('Dra. Renata', '1976-10-22', '888.999.000-11', '888999000111', 'Dra. R', '23456-789', 'Avenida N, 987', 'Cidade J', 'UF', 'Bairro J', '(11) 4321-9876', 67891, 'RJ', 'A');</t>
-  </si>
-  <si>
-    <t>-- Inserir 5 especialidades</t>
-  </si>
-  <si>
-    <t>INSERT INTO especialidade (esp_nome_especialidade, esp_codigo_especialidade, esp_ativo)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    ('Cardiologia', 1, 'A'),</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    ('Pediatria', 2, 'A'),</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    ('Ortopedia', 3, 'A'),</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    ('Dermatologia', 4, 'A'),</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    ('Ginecologia', 5, 'A');</t>
-  </si>
-  <si>
-    <t>INSERT INTO medico_especialidade (fk_med_id, fk_esp_id, med_esp_ativo)</t>
-  </si>
-  <si>
-    <t>-- Inserir 5 convênios</t>
-  </si>
-  <si>
-    <t>INSERT INTO convenio (con_nome_convenio, con_tipo_plano, con_fone, con_ativo)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    ('Plano de Saúde A', 'P1', '(11) 1234-5678', 'A'),</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    ('Plano de Saúde B', 'P2', '(22) 9876-5432', 'A'),</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    ('Plano de Saúde C', 'P3', '(33) 6543-2109', 'A'),</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    ('Plano de Saúde D', 'P4', '(44) 1098-7654', 'A'),</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    ('Plano de Saúde E', 'P5', '(55) 4321-0987', 'A');</t>
-  </si>
-  <si>
-    <t>-- Inserir 5 pacientes</t>
-  </si>
-  <si>
-    <t>INSERT INTO paciente (pac_nome, pac_datanasc, pac_cpf, pac_rg, pac_sexo, pac_estado_civil, pac_endereco, pac_cidade, pac_bairro, pac_cep, pac_fone, pac_nome_mae, pac_nome_pai, pac_responsavel, fk_con_id, pac_ativo)</t>
-  </si>
-  <si>
-    <t>-- Inserir 10 consultas para um paciente</t>
-  </si>
-  <si>
-    <t>INSERT INTO mov_consulta_paciente (fk_pac_prontuario, fk_med_id, fk_esp_id, fk_con_id, mov_data_atende, mov_hora_atende, mov_ativo, mov_evolucao_medica)</t>
-  </si>
-  <si>
-    <t>-- Inserir 1 consulta isolada para outro paciente</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> --Associar especialidades aos médicos (pode haver mais de uma especialidade para um médico)</t>
-  </si>
-  <si>
     <t>SELECT m.med_nome AS medico, e.esp_nome_especialidade AS especialidade</t>
   </si>
   <si>
@@ -220,90 +124,6 @@
     <t>select * from convenio</t>
   </si>
   <si>
-    <t xml:space="preserve">    (21, 11, 'A'),</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    (21, 12, 'A'),</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    (22, 11, 'A'),</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    (23, 13, 'A'),</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    (23, 14, 'A'),</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    (24, 15, 'A'),</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    (25, 11, 'A'),</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    (26, 12, 'A'),</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    (27, 13, 'A'),</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    (28, 14, 'A');</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    ('Fernanda', '1993-07-20', '111.222.333-44', '111222333444', 'F', 'Solteira', 'Rua X, 789', 'Cidade C', 'Bairro C', '87654-321', '(11) 7654-3210', 'Mãe Fernanda', 'Pai João', 'Responsável 1', 6, 'A'),</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    ('Rafael', '1988-03-12', '555.666.777-88', '555666777888', 'M', 'Casado', 'Rua Y, 987', 'Cidade D', 'Bairro D', '56789-012', '(22) 5432-1098', 'Mãe Rafaela', 'Pai José', 'Responsável 2', 7, 'A'),</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    ('Luciana', '1990-05-15', '777.888.999-00', '777888999000', 'F', 'Solteira', 'Rua Z, 543', 'Cidade E', 'Bairro E', '34567-890', '(22) 4321-9876', 'Mãe Luciana', 'Pai Roberto', 'Responsável 3', 8, 'A'),</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    ('Felipe', '1985-11-25', '999.000.111-22', '999000111222', 'M', 'Casado', 'Avenida W, 876', 'Cidade F', 'Bairro F', '23456-789', '(11) 8765-4321', 'Mãe Felipe', 'Pai Marcos', 'Responsável 4', 9, 'A'),</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    ('Camila', '1972-09-30', '333.444.555-66', '333444555666', 'F', 'Solteira', 'Rua K, 123', 'Cidade G', 'Bairro G', '54321-876', '(11) 5432-1098', 'Mãe Camila', 'Pai Ricardo', 'Responsável 5', 10, 'A');</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    (16, 21, 11, 6, '2023-01-15', '12:30:00', 'A', 'Consulta de rotina. Paciente está saudável.'),</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    (16, 22, 12, 6, '2023-02-20', '14:00:00', 'A', 'Consulta pediátrica. Sem problemas detectados.'),</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    (16, 23, 13, 6, '2023-03-10', '10:00:00', 'A', 'Consulta ortopédica. Recomendado repouso.'),</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    (16, 24, 14, 7, '2023-04-05', '11:30:00', 'A', 'Consulta dermatológica. Tratamento indicado.'),</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    (16, 25, 15, 7, '2023-05-20', '15:45:00', 'A', 'Consulta ginecológica. Sem alterações.'),</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    (16, 21, 11, 8, '2023-06-15', '09:00:00', 'A', 'Consulta de retorno. Paciente está estável.'),</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    (16, 22, 12, 9, '2023-07-10', '13:30:00', 'A', 'Consulta de rotina. Tudo dentro da normalidade.'),</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    (16, 23, 13, 6, '2023-08-25', '16:15:00', 'A', 'Consulta ortopédica. Recomendado fisioterapia.'),</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    (16, 24, 14, 6, '2023-09-18', '10:45:00', 'A', 'Consulta dermatológica. Tratamento em curso.'),</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    (16, 25, 15, 6, '2023-10-12', '14:20:00', 'A', 'Consulta ginecológica. Sem complicações.');</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    (17,21,11, 6, '2023-11-08', '11:02:00', 'A', 'Consulta cardiológica. Resultados normais.');</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    (18, 21, 11, 8, '2023-11-08', '11:02:00', 'A', 'Consultation for cardiac issues. Normal results.'),</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    (19, 22, 12, 9, '2023-11-09', '14:30:00', 'A', 'Dermatology consultation. Prescription provided.');</t>
-  </si>
-  <si>
     <t>CREATE TABLE "medico" (</t>
   </si>
   <si>
@@ -376,24 +196,12 @@
     <t xml:space="preserve">  "pac_datanasc" DATE NOT NULL,</t>
   </si>
   <si>
-    <t xml:space="preserve">  "pac_endereco" VARCHAR(100),</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "pac_cidade" VARCHAR(50),</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "pac_bairro" VARCHAR(50),</t>
-  </si>
-  <si>
     <t xml:space="preserve">  "pac_nome_mae" VARCHAR(100),</t>
   </si>
   <si>
     <t xml:space="preserve">  "pac_nome_pai" VARCHAR(100),</t>
   </si>
   <si>
-    <t xml:space="preserve">  "pac_responsavel" VARCHAR(100) NOT NULL,</t>
-  </si>
-  <si>
     <t xml:space="preserve">  "fk_con_id" INT NOT NULL,</t>
   </si>
   <si>
@@ -427,9 +235,6 @@
     <t xml:space="preserve">  "med_uf_medico" CHAR(2),</t>
   </si>
   <si>
-    <t xml:space="preserve">  "med_fone" CHAR(20) NOT NULL,</t>
-  </si>
-  <si>
     <t xml:space="preserve">  "med_ativo" CHAR(1)</t>
   </si>
   <si>
@@ -448,9 +253,6 @@
     <t xml:space="preserve">  "con_tipo_plano" CHAR(3) NOT NULL,</t>
   </si>
   <si>
-    <t xml:space="preserve">  "con_fone" CHAR(20) NOT NULL,</t>
-  </si>
-  <si>
     <t xml:space="preserve">  "con_ativo" CHAR(1)</t>
   </si>
   <si>
@@ -460,18 +262,9 @@
     <t xml:space="preserve">  "pac_rg" CHAR(12),</t>
   </si>
   <si>
-    <t xml:space="preserve">  "pac_sexo" CHAR(1) NOT NULL,</t>
-  </si>
-  <si>
     <t xml:space="preserve">  "pac_estado_civil" CHAR(15),</t>
   </si>
   <si>
-    <t xml:space="preserve">  "pac_cep" CHAR(10),</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "pac_fone" CHAR(20) NOT NULL,</t>
-  </si>
-  <si>
     <t xml:space="preserve">  "pac_ativo" CHAR(1),</t>
   </si>
   <si>
@@ -497,6 +290,252 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "pac_genero" CHAR(10) NOT NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "med_fone" VARCHAR(20) NOT NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "con_fone" VARCHAR(20) NOT NULL, -- Change CHAR to VARCHAR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "pac_nome_social" VARCHAR(100),</t>
+  </si>
+  <si>
+    <t>CREATE TABLE pac_endereco (</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  CONSTRAINT "fk_pac_endereco_paciente" FOREIGN KEY ("fk_pac_prontuario") REFERENCES "paciente" ("pac_prontuario")</t>
+  </si>
+  <si>
+    <t>CREATE TABLE pac_informacao (</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  CONSTRAINT "fk_pac_informacao_paciente" FOREIGN KEY ("fk_pac_prontuario") REFERENCES "paciente" ("pac_prontuario")</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "pac_inf_responsavel" VARCHAR(100),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  pac_inf_id SERIAL PRIMARY KEY, -- Change "pac_id_informaca" to "pac_id_informacao"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "pac_end_endereco" VARCHAR(100),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "pac_end_cidade" VARCHAR(50),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "pac_end_bairro" VARCHAR(50),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "pac_end_cep" CHAR(10),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "pac_end_id" SERIAL PRIMARY KEY,</t>
+  </si>
+  <si>
+    <t>-- Inserting data into the "medico" table</t>
+  </si>
+  <si>
+    <t>INSERT INTO "medico" ("med_nome", "med_datanasc", "med_cpf", "med_rg", "med_apelido", "med_cep", "med_endereco", "med_cidade", "med_uf_medico", "med_bairro", "med_fone", "med_crm", "med_uf_crm", "med_ativo")</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ('Dr. Smith', '1980-01-01', '12345678901234', '123456789012', 'Doc', '12345-678', '123 Main St', 'City', 'CA', 'Suburb', '555-1234', 987654, 'CA', '1'),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ('Dr. Johnson', '1975-03-15', '98765432109876', '987654321098', 'Dr. J', '54321-876', '456 Oak St', 'Town', 'NY', 'Downtown', '555-5678', 654321, 'NY', '1'),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ('Dr. Williams', '1988-05-20', '45678901234567', '456789012345', 'Will', '98765-432', '789 Elm St', 'Village', 'TX', 'Uptown', '555-9876', 123456, 'TX', '1'),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ('Dr. Davis', '1982-08-10', '78901234567890', '789012345678', 'Dav', '23456-789', '012 Maple St', 'Hamlet', 'FL', 'Rural', '555-5432', 234567, 'FL', '1'),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ('Dr. Miller', '1990-12-05', '23456789012345', '234567890123', 'Mil', '87654-321', '789 Pine St', 'City', 'WA', 'Hill', '555-8765', 876543, 'WA', '1');</t>
+  </si>
+  <si>
+    <t>-- Inserting data into the "especialidade" table</t>
+  </si>
+  <si>
+    <t>INSERT INTO "especialidade" ("esp_nome_especialidade", "esp_codigo_especialidade", "esp_ativo")</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ('Cardiologia', 101, '1'),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ('Dermatologia', 102, '1'),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ('Ortopedia', 103, '1'),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ('Ginecologia', 104, '1'),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ('Pediatria', 105, '1');</t>
+  </si>
+  <si>
+    <t>-- Inserting data into the "medico_especialidade" table</t>
+  </si>
+  <si>
+    <t>INSERT INTO "medico_especialidade" ("fk_med_id", "fk_esp_id", "med_esp_ativo")</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  (1, 1, '1'),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  (1, 3, '1'),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  (2, 2, '1'),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  (2, 4, '1'),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  (3, 1, '1'),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  (3, 5, '1'),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  (4, 3, '1'),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  (4, 5, '1'),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  (5, 2, '1'),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  (5, 4, '1');</t>
+  </si>
+  <si>
+    <t>-- Inserting data into the "convenio" table</t>
+  </si>
+  <si>
+    <t>INSERT INTO "convenio" ("con_nome_convenio", "con_tipo_plano", "con_fone", "con_ativo")</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ('HealthCare Plus', 'PPO', '800-123-4567', '1'),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ('MedicalCare', 'HMO', '888-987-6543', '1'),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ('Wellness Insurance', 'POS', '877-654-3210', '1'),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ('Flex Health', 'HDHP', '866-234-5678', '1'),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ('Family Health Plan', 'EPO', '855-876-5432', '1');</t>
+  </si>
+  <si>
+    <t>-- Inserting data into the "paciente" table</t>
+  </si>
+  <si>
+    <t>INSERT INTO "paciente" ("pac_nome", "pac_nome_social", "pac_datanasc", "pac_cpf", "pac_rg", "pac_genero", "pac_estado_civil", "pac_fone", "pac_nome_mae", "pac_nome_pai", "fk_con_id", "pac_ativo")</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ('John Doe', 'Johnny', '1995-02-20', '11122233344455', '123456789012', 'Male', 'Single', '555-1111', 'Mary Doe', 'Bob Doe', 1, '1'),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ('Jane Smith', NULL, '1988-07-12', '22233344455566', '234567890123', 'Female', 'Married', '555-2222', 'Emily Smith', 'Tom Smith', 2, '1'),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ('Mike Johnson', NULL, '1970-09-05', '33344455566677', '345678901234', 'Male', 'Divorced', '555-3333', 'Susan Johnson', NULL, 3, '1'),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ('Emily Williams', 'Em', '1985-12-30', '44455566677788', '456789012345', 'Female', 'Widowed', '555-4444', NULL, 'David Williams', 4, '1'),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ('Chris Davis', NULL, '2000-04-15', '55566677788899', '567890123456', 'Non-Binary', 'Single', '555-5555', 'Pat Davis', NULL, 5, '1');</t>
+  </si>
+  <si>
+    <t>-- Inserting data into the "pac_endereco" table</t>
+  </si>
+  <si>
+    <t>INSERT INTO "pac_endereco" ("pac_end_endereco", "pac_end_cidade", "pac_end_bairro", "pac_end_cep", "fk_pac_prontuario")</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ('456 Oak St', 'Town', 'Downtown', '54321-876', 2),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ('789 Elm St', 'Village', 'Uptown', '98765-432', 3),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ('012 Maple St', 'Hamlet', 'Rural', '23456-789', 4),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ('789 Pine St', 'City', 'Hill', '87654-321', 5),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ('456 Main St', 'Metropolis', 'Downtown', '65432-109', 1);</t>
+  </si>
+  <si>
+    <t>-- Inserting data into the "pac_informacao" table</t>
+  </si>
+  <si>
+    <t>INSERT INTO "pac_informacao" ("pac_inf_responsavel", "pac_inf_fone", "fk_pac_prontuario")</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ('Mary Doe', '555-1111', 1),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ('Emily Smith', '555-2222', 2),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ('Susan Johnson', '555-3333', 3),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  (NULL, '555-4444', 4),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ('Pat Davis', '555-5555', 5);</t>
+  </si>
+  <si>
+    <t>-- Inserting data into the "mov_consulta_paciente" table</t>
+  </si>
+  <si>
+    <t>INSERT INTO "mov_consulta_paciente" ("fk_pac_prontuario", "fk_med_id", "fk_esp_id", "fk_con_id", "mov_data_atende", "mov_hora_atende", "mov_ativo", "mov_evolucao_medica")</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  (1, 1, 1, 1, '2023-11-23', '09:00', '1', 'Routine check-up'),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  (2, 2, 2, 2, '2023-11-24', '10:30', '1', 'Skin examination'),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  (3, 3, 3, 3, '2023-11-25', '11:45', '1', 'Orthopedic consultation'),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  (4, 4, 4, 4, '2023-11-26', '13:15', '1', 'Gynecological exam'),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  (5, 5, 5, 5, '2023-11-27', '14:30', '1', 'Pediatric check-up'),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  (1, 2, 3, 4, '2023-11-28', '15:45', '1', 'Complex consultation'),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  (2, 3, 4, 5, '2023-11-29', '16:30', '1', 'Follow-up appointment'),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  (3, 4, 5, 1, '2023-11-30', '17:15', '1', 'Emergency visit'),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  (4, 5, 1, 2, '2023-12-01', '18:00', '1', 'Pediatric consultation'),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  (5, 1, 2, 3, '2023-12-02', '19:00', '1', 'Cardiology check-up');</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "pac_inf_fone" VARCHAR(20) NOT NULL, </t>
   </si>
 </sst>
 </file>
@@ -879,10 +918,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1A0769B-AFF5-42E8-9E44-814946580095}">
-  <dimension ref="A1:D87"/>
+  <dimension ref="A1:D100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="A97" sqref="A97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -901,87 +940,87 @@
     </row>
     <row r="2" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>152</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>88</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>89</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>90</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>91</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>124</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>125</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>126</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>127</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>92</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>93</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>128</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>94</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>129</v>
+        <v>85</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>95</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>96</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>130</v>
+        <v>65</v>
       </c>
     </row>
     <row r="19" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
@@ -994,27 +1033,27 @@
     </row>
     <row r="21" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>97</v>
+        <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>98</v>
+        <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>99</v>
+        <v>39</v>
       </c>
     </row>
     <row r="24" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>100</v>
+        <v>40</v>
       </c>
     </row>
     <row r="25" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>131</v>
+        <v>66</v>
       </c>
     </row>
     <row r="26" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
@@ -1027,37 +1066,37 @@
     </row>
     <row r="28" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>101</v>
+        <v>41</v>
       </c>
     </row>
     <row r="29" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>102</v>
+        <v>42</v>
       </c>
     </row>
     <row r="30" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>103</v>
+        <v>43</v>
       </c>
     </row>
     <row r="31" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>104</v>
+        <v>44</v>
       </c>
     </row>
     <row r="32" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>132</v>
+        <v>67</v>
       </c>
     </row>
     <row r="33" spans="1:2" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>133</v>
+        <v>68</v>
       </c>
     </row>
     <row r="34" spans="1:2" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>134</v>
+        <v>69</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
@@ -1070,32 +1109,32 @@
     </row>
     <row r="37" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>105</v>
+        <v>45</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>106</v>
+        <v>46</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>107</v>
+        <v>47</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>135</v>
+        <v>70</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>136</v>
+        <v>86</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>137</v>
+        <v>71</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
@@ -1108,203 +1147,265 @@
     </row>
     <row r="45" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>108</v>
+        <v>48</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
-        <v>109</v>
+        <v>49</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
-        <v>110</v>
+        <v>50</v>
       </c>
       <c r="B47" s="1"/>
     </row>
-    <row r="48" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A48" s="3" t="s">
-        <v>111</v>
-      </c>
+    <row r="48" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A48" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B48" s="1"/>
     </row>
     <row r="49" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>138</v>
+        <v>51</v>
       </c>
     </row>
     <row r="50" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>139</v>
+        <v>72</v>
       </c>
     </row>
     <row r="51" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>140</v>
+        <v>73</v>
       </c>
     </row>
     <row r="52" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>141</v>
+        <v>84</v>
       </c>
     </row>
     <row r="53" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>112</v>
+        <v>74</v>
       </c>
     </row>
     <row r="54" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>113</v>
+        <v>52</v>
       </c>
     </row>
     <row r="55" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>114</v>
+        <v>53</v>
       </c>
     </row>
     <row r="56" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
-        <v>142</v>
+        <v>54</v>
       </c>
     </row>
     <row r="57" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>143</v>
+        <v>75</v>
       </c>
     </row>
     <row r="58" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>115</v>
+        <v>76</v>
       </c>
     </row>
     <row r="59" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>116</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A60" s="3" t="s">
-        <v>117</v>
-      </c>
+      <c r="A60" s="3"/>
     </row>
     <row r="61" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
-        <v>118</v>
+        <v>88</v>
       </c>
     </row>
     <row r="62" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
-        <v>144</v>
+        <v>98</v>
       </c>
     </row>
     <row r="63" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
-        <v>145</v>
+        <v>94</v>
       </c>
     </row>
     <row r="64" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
-        <v>1</v>
+        <v>95</v>
       </c>
     </row>
     <row r="65" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A65" s="3"/>
+      <c r="A65" s="3" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="66" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
-        <v>119</v>
+        <v>97</v>
       </c>
     </row>
     <row r="67" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
-        <v>120</v>
+        <v>57</v>
       </c>
     </row>
     <row r="68" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A69" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="70" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A70" s="2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="71" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A71" s="2" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="72" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A72" s="2" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="73" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A73" s="2" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="74" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A74" s="2" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="75" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A75" s="2" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="76" spans="1:1" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A69" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A70" s="3"/>
+    </row>
+    <row r="71" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A71" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A72" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A73" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A74" s="3" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A75" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
-        <v>148</v>
+        <v>91</v>
       </c>
     </row>
     <row r="77" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
-        <v>149</v>
+        <v>1</v>
       </c>
     </row>
     <row r="78" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A78" s="3" t="s">
-        <v>150</v>
-      </c>
+      <c r="A78" s="3"/>
     </row>
     <row r="79" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="80" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A80" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A80" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A81" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A82" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A83" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A84" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A85" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A86" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A87" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A88" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A89" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A90" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A91" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A92" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A93" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A81" s="2"/>
-    </row>
-    <row r="82" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A82" s="2"/>
-    </row>
-    <row r="83" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A83" s="3"/>
-    </row>
-    <row r="84" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A84" s="2"/>
-    </row>
-    <row r="85" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A85" s="2"/>
-    </row>
-    <row r="86" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A86" s="2"/>
-    </row>
-    <row r="87" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A87" s="2"/>
+    <row r="94" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A94" s="2"/>
+    </row>
+    <row r="95" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A95" s="2"/>
+    </row>
+    <row r="96" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A96" s="3"/>
+    </row>
+    <row r="97" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A97" s="2"/>
+    </row>
+    <row r="98" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A98" s="2"/>
+    </row>
+    <row r="99" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A99" s="2"/>
+    </row>
+    <row r="100" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A100" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1317,9 +1418,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D84C294C-2FC1-49D3-B99F-6F427703C9D2}">
-  <dimension ref="A1:A79"/>
+  <dimension ref="A1:A83"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1331,354 +1434,374 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-    </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>101</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>103</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>104</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>12</v>
+        <v>105</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>106</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>107</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>108</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>109</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>4</v>
+        <v>110</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>111</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>19</v>
+        <v>112</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>113</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>114</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>35</v>
+        <v>115</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>22</v>
+        <v>116</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>4</v>
+        <v>117</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>60</v>
+        <v>118</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>61</v>
+        <v>119</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>62</v>
+        <v>120</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>63</v>
+        <v>121</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>64</v>
+        <v>122</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>65</v>
+        <v>123</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>67</v>
+        <v>124</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>68</v>
+        <v>125</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>69</v>
+        <v>126</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>23</v>
+        <v>127</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>24</v>
+        <v>128</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>4</v>
+        <v>129</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>25</v>
+        <v>130</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>27</v>
+        <v>131</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>28</v>
+        <v>132</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>29</v>
+        <v>133</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>30</v>
+        <v>134</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>31</v>
+        <v>135</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>4</v>
+        <v>136</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>70</v>
+        <v>137</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>72</v>
+        <v>138</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>73</v>
+        <v>139</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>74</v>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>32</v>
+        <v>141</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>33</v>
+        <v>142</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>4</v>
+        <v>143</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>75</v>
+        <v>144</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>77</v>
+        <v>145</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>78</v>
+        <v>146</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>79</v>
+        <v>147</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>80</v>
+        <v>3</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>81</v>
+        <v>148</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>82</v>
+        <v>149</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>83</v>
+        <v>150</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>34</v>
+        <v>151</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>33</v>
+        <v>153</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>4</v>
+        <v>154</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>85</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>33</v>
+        <v>157</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>4</v>
+        <v>158</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>86</v>
+        <v>159</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>87</v>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -1701,122 +1824,122 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>52</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>53</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>54</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>55</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>56</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>57</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>58</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>59</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>44</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>36</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>38</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>39</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>43</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>40</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>41</v>
+        <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>51</v>
+        <v>19</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>45</v>
+        <v>13</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>46</v>
+        <v>14</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>47</v>
+        <v>15</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>48</v>
+        <v>16</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>50</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>